<commit_message>
Completed ServiceRequest Pathology Order in Diagnostic Report FHIR IG
Fixes #31
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/servicerequest-path-report-1.xlsx
+++ b/output/DiagnosticReport/servicerequest-path-report-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2446" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="500">
   <si>
     <t>Path</t>
   </si>
@@ -160,7 +160,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}prr-1:orderDetail SHALL only be present if code is present {orderDetail.empty() or code.exists()}</t>
+dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}prr-1:orderDetail SHALL only be present if code is present {orderDetail.empty() or code.exists()}inv-dh-prr-01:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-prr-02:The requester shall at least have a reference or an identifier with at least a system and a value {requester.reference.exists() or requester.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Request</t>
@@ -797,7 +797,7 @@
     <t>ServiceRequest.status</t>
   </si>
   <si>
-    <t>draft | active | on-hold | revoked | completed | entered-in-error | unknown</t>
+    <t>active | on-hold | completed</t>
   </si>
   <si>
     <t>The status of the order.</t>
@@ -806,10 +806,7 @@
     <t>The status is generally fully in the control of the requester - they determine whether the order is draft or active and, after it has been activated, competed, cancelled or suspended. States relating to the activities of the performer are reflected on either the corresponding event (see [Event Pattern](http://hl7.org/fhir/R4/event.html) for general discussion) or using the [Task](http://hl7.org/fhir/R4/task.html) resource.</t>
   </si>
   <si>
-    <t>The status of a service order.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/request-status|4.0.1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/requeststatus-reporting-1</t>
   </si>
   <si>
     <t>Request.status</t>
@@ -969,10 +966,10 @@
     <t>Many laboratory and radiology procedure codes embed the specimen/organ system in the test order name, for example,  serum or serum/plasma glucose, or a chest x-ray. The specimen might not be recorded separately from the test code.</t>
   </si>
   <si>
-    <t>Codes for tests or services that can be carried out by a designated individual, organization or healthcare service.  For laboratory, LOINC is  (preferred)[http://build.fhir.org/terminologies.html#preferred] and a valueset using LOINC Order codes is available [here](valueset-diagnostic-requests.html).</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/procedure-code</t>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/pathology-procedure-1</t>
   </si>
   <si>
     <t>Request.code</t>
@@ -1066,7 +1063,7 @@
     <t>ServiceRequest.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/patient-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-mhr-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/patient-ident-1)
 </t>
   </si>
   <si>
@@ -1219,7 +1216,7 @@
 orderer</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/practitionerrole-ident-1|http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-ident-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/practitionerrole-ident-1|http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-ident-1)
 </t>
   </si>
   <si>
@@ -1767,8 +1764,8 @@
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="66.81640625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="122.19921875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="69.17578125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>
@@ -5270,11 +5267,9 @@
       <c r="W31" t="s" s="2">
         <v>145</v>
       </c>
-      <c r="X31" t="s" s="2">
+      <c r="X31" s="2"/>
+      <c r="Y31" t="s" s="2">
         <v>252</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>253</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>44</v>
@@ -5307,24 +5302,24 @@
         <v>64</v>
       </c>
       <c r="AJ31" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AK31" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="AK31" t="s" s="2">
+      <c r="AL31" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="AL31" t="s" s="2">
+      <c r="AM31" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="AM31" t="s" s="2">
+      <c r="AN31" t="s" s="2">
         <v>257</v>
-      </c>
-      <c r="AN31" t="s" s="2">
-        <v>258</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5350,13 +5345,13 @@
         <v>72</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="L32" t="s" s="2">
+      <c r="M32" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -5364,7 +5359,7 @@
       </c>
       <c r="P32" s="2"/>
       <c r="Q32" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="R32" t="s" s="2">
         <v>44</v>
@@ -5385,11 +5380,11 @@
         <v>145</v>
       </c>
       <c r="X32" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="Y32" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="Y32" t="s" s="2">
-        <v>265</v>
-      </c>
       <c r="Z32" t="s" s="2">
         <v>44</v>
       </c>
@@ -5406,7 +5401,7 @@
         <v>44</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>52</v>
@@ -5421,16 +5416,16 @@
         <v>64</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>95</v>
       </c>
       <c r="AL32" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="AM32" t="s" s="2">
-        <v>268</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>44</v>
@@ -5438,7 +5433,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5464,16 +5459,16 @@
         <v>151</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="L33" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="L33" t="s" s="2">
+      <c r="M33" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="M33" t="s" s="2">
+      <c r="N33" t="s" s="2">
         <v>272</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>273</v>
       </c>
       <c r="O33" t="s" s="2">
         <v>44</v>
@@ -5483,29 +5478,29 @@
         <v>44</v>
       </c>
       <c r="R33" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="S33" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T33" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U33" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V33" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W33" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="S33" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="W33" t="s" s="2">
+      <c r="X33" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="X33" t="s" s="2">
+      <c r="Y33" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="Y33" t="s" s="2">
-        <v>277</v>
-      </c>
       <c r="Z33" t="s" s="2">
         <v>44</v>
       </c>
@@ -5522,7 +5517,7 @@
         <v>44</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>42</v>
@@ -5540,13 +5535,13 @@
         <v>44</v>
       </c>
       <c r="AK33" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="AL33" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="AL33" t="s" s="2">
-        <v>279</v>
-      </c>
       <c r="AM33" t="s" s="2">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>44</v>
@@ -5554,7 +5549,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5580,10 +5575,10 @@
         <v>72</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L34" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -5591,7 +5586,7 @@
         <v>44</v>
       </c>
       <c r="P34" t="s" s="2">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Q34" t="s" s="2">
         <v>44</v>
@@ -5615,11 +5610,11 @@
         <v>145</v>
       </c>
       <c r="X34" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Y34" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="Y34" t="s" s="2">
-        <v>285</v>
-      </c>
       <c r="Z34" t="s" s="2">
         <v>44</v>
       </c>
@@ -5636,7 +5631,7 @@
         <v>44</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>42</v>
@@ -5651,16 +5646,16 @@
         <v>64</v>
       </c>
       <c r="AJ34" t="s" s="2">
+        <v>285</v>
+      </c>
+      <c r="AK34" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="AK34" t="s" s="2">
+      <c r="AL34" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="AL34" t="s" s="2">
+      <c r="AM34" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>44</v>
@@ -5668,7 +5663,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5691,26 +5686,26 @@
         <v>53</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>290</v>
+      </c>
+      <c r="K35" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="K35" t="s" s="2">
+      <c r="L35" t="s" s="2">
         <v>292</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="N35" t="s" s="2">
+      <c r="O35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P35" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="O35" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="P35" t="s" s="2">
-        <v>296</v>
-      </c>
       <c r="Q35" t="s" s="2">
         <v>44</v>
       </c>
@@ -5754,7 +5749,7 @@
         <v>44</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>42</v>
@@ -5769,13 +5764,13 @@
         <v>64</v>
       </c>
       <c r="AJ35" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL35" t="s" s="2">
         <v>297</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL35" t="s" s="2">
-        <v>298</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>44</v>
@@ -5786,11 +5781,11 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
@@ -5812,13 +5807,13 @@
         <v>151</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="L36" t="s" s="2">
+      <c r="M36" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
@@ -5844,14 +5839,12 @@
         <v>44</v>
       </c>
       <c r="W36" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="X36" t="s" s="2">
+        <v>303</v>
+      </c>
+      <c r="X36" s="2"/>
+      <c r="Y36" t="s" s="2">
         <v>304</v>
       </c>
-      <c r="Y36" t="s" s="2">
-        <v>305</v>
-      </c>
       <c r="Z36" t="s" s="2">
         <v>44</v>
       </c>
@@ -5868,7 +5861,7 @@
         <v>44</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>42</v>
@@ -5883,24 +5876,24 @@
         <v>64</v>
       </c>
       <c r="AJ36" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="AK36" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="AK36" t="s" s="2">
+      <c r="AL36" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="AL36" t="s" s="2">
+      <c r="AM36" t="s" s="2">
         <v>308</v>
       </c>
-      <c r="AM36" t="s" s="2">
+      <c r="AN36" t="s" s="2">
         <v>309</v>
-      </c>
-      <c r="AN36" t="s" s="2">
-        <v>310</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -6012,7 +6005,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -6126,7 +6119,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6198,7 +6191,7 @@
         <v>44</v>
       </c>
       <c r="AA39" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AB39" s="2"/>
       <c r="AC39" t="s" s="2">
@@ -6240,10 +6233,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C40" t="s" s="2">
         <v>44</v>
@@ -6268,7 +6261,7 @@
         <v>162</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L40" t="s" s="2">
         <v>164</v>
@@ -6306,7 +6299,7 @@
       </c>
       <c r="X40" s="2"/>
       <c r="Y40" t="s" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>44</v>
@@ -6356,7 +6349,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6472,11 +6465,11 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" t="s" s="2">
@@ -6498,13 +6491,13 @@
         <v>151</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>321</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6530,14 +6523,14 @@
         <v>44</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X42" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="Y42" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="Y42" t="s" s="2">
-        <v>325</v>
-      </c>
       <c r="Z42" t="s" s="2">
         <v>44</v>
       </c>
@@ -6554,7 +6547,7 @@
         <v>44</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>42</v>
@@ -6563,7 +6556,7 @@
         <v>43</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AI42" t="s" s="2">
         <v>64</v>
@@ -6572,21 +6565,21 @@
         <v>44</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6609,17 +6602,17 @@
         <v>53</v>
       </c>
       <c r="J43" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="K43" t="s" s="2">
         <v>329</v>
       </c>
-      <c r="K43" t="s" s="2">
+      <c r="L43" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>331</v>
       </c>
       <c r="M43" s="2"/>
       <c r="N43" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>44</v>
@@ -6668,7 +6661,7 @@
         <v>44</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>42</v>
@@ -6686,10 +6679,10 @@
         <v>44</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>44</v>
@@ -6700,7 +6693,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6723,13 +6716,13 @@
         <v>53</v>
       </c>
       <c r="J44" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="K44" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="K44" t="s" s="2">
+      <c r="L44" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" s="2"/>
@@ -6780,7 +6773,7 @@
         <v>44</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>52</v>
@@ -6795,28 +6788,28 @@
         <v>64</v>
       </c>
       <c r="AJ44" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="AK44" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="AK44" t="s" s="2">
+      <c r="AL44" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="AL44" t="s" s="2">
+      <c r="AM44" t="s" s="2">
         <v>340</v>
       </c>
-      <c r="AM44" t="s" s="2">
+      <c r="AN44" t="s" s="2">
         <v>341</v>
-      </c>
-      <c r="AN44" t="s" s="2">
-        <v>342</v>
       </c>
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
@@ -6835,13 +6828,13 @@
         <v>53</v>
       </c>
       <c r="J45" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="K45" t="s" s="2">
         <v>345</v>
       </c>
-      <c r="K45" t="s" s="2">
+      <c r="L45" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="L45" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6892,7 +6885,7 @@
         <v>44</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>42</v>
@@ -6907,28 +6900,28 @@
         <v>64</v>
       </c>
       <c r="AJ45" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="AK45" t="s" s="2">
         <v>348</v>
       </c>
-      <c r="AK45" t="s" s="2">
+      <c r="AL45" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="AL45" t="s" s="2">
+      <c r="AM45" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="AM45" t="s" s="2">
+      <c r="AN45" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="AN45" t="s" s="2">
-        <v>352</v>
       </c>
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6947,13 +6940,13 @@
         <v>53</v>
       </c>
       <c r="J46" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="K46" t="s" s="2">
         <v>355</v>
       </c>
-      <c r="K46" t="s" s="2">
+      <c r="L46" t="s" s="2">
         <v>356</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>357</v>
       </c>
       <c r="M46" s="2"/>
       <c r="N46" s="2"/>
@@ -7004,7 +6997,7 @@
         <v>44</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>42</v>
@@ -7019,24 +7012,24 @@
         <v>64</v>
       </c>
       <c r="AJ46" t="s" s="2">
+        <v>357</v>
+      </c>
+      <c r="AK46" t="s" s="2">
         <v>358</v>
       </c>
-      <c r="AK46" t="s" s="2">
+      <c r="AL46" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="AL46" t="s" s="2">
+      <c r="AM46" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="AM46" t="s" s="2">
+      <c r="AN46" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="AN46" t="s" s="2">
-        <v>362</v>
       </c>
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -7059,13 +7052,13 @@
         <v>53</v>
       </c>
       <c r="J47" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="K47" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="K47" t="s" s="2">
+      <c r="L47" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -7092,14 +7085,14 @@
         <v>44</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X47" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="Y47" t="s" s="2">
         <v>367</v>
       </c>
-      <c r="Y47" t="s" s="2">
-        <v>368</v>
-      </c>
       <c r="Z47" t="s" s="2">
         <v>44</v>
       </c>
@@ -7116,7 +7109,7 @@
         <v>44</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>42</v>
@@ -7137,22 +7130,22 @@
         <v>44</v>
       </c>
       <c r="AL47" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN47" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>370</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
@@ -7171,13 +7164,13 @@
         <v>53</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>372</v>
+      </c>
+      <c r="K48" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="K48" t="s" s="2">
+      <c r="L48" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -7228,7 +7221,7 @@
         <v>44</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>42</v>
@@ -7243,28 +7236,28 @@
         <v>64</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="AK48" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="AK48" t="s" s="2">
+      <c r="AL48" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="AL48" t="s" s="2">
+      <c r="AM48" t="s" s="2">
         <v>378</v>
       </c>
-      <c r="AM48" t="s" s="2">
+      <c r="AN48" t="s" s="2">
         <v>379</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>380</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
@@ -7283,16 +7276,16 @@
         <v>53</v>
       </c>
       <c r="J49" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="K49" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="K49" t="s" s="2">
+      <c r="L49" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
@@ -7342,7 +7335,7 @@
         <v>44</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>42</v>
@@ -7357,28 +7350,28 @@
         <v>64</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AK49" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="AK49" t="s" s="2">
+      <c r="AL49" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="AL49" t="s" s="2">
+      <c r="AM49" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="AM49" t="s" s="2">
+      <c r="AN49" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="AN49" t="s" s="2">
-        <v>391</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -7400,13 +7393,13 @@
         <v>151</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>395</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>396</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
@@ -7432,14 +7425,14 @@
         <v>44</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X50" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="Y50" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="Y50" t="s" s="2">
-        <v>398</v>
-      </c>
       <c r="Z50" t="s" s="2">
         <v>44</v>
       </c>
@@ -7456,7 +7449,7 @@
         <v>44</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>42</v>
@@ -7471,16 +7464,16 @@
         <v>64</v>
       </c>
       <c r="AJ50" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="AK50" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="AK50" t="s" s="2">
+      <c r="AL50" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="AL50" t="s" s="2">
+      <c r="AM50" t="s" s="2">
         <v>401</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>402</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>44</v>
@@ -7488,7 +7481,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7600,7 +7593,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7714,7 +7707,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7786,7 +7779,7 @@
         <v>44</v>
       </c>
       <c r="AA53" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AB53" s="2"/>
       <c r="AC53" t="s" s="2">
@@ -7828,10 +7821,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C54" t="s" s="2">
         <v>44</v>
@@ -7856,7 +7849,7 @@
         <v>162</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L54" t="s" s="2">
         <v>164</v>
@@ -7894,7 +7887,7 @@
       </c>
       <c r="X54" s="2"/>
       <c r="Y54" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>44</v>
@@ -7944,10 +7937,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C55" t="s" s="2">
         <v>44</v>
@@ -7972,7 +7965,7 @@
         <v>162</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L55" t="s" s="2">
         <v>164</v>
@@ -8010,7 +8003,7 @@
       </c>
       <c r="X55" s="2"/>
       <c r="Y55" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Z55" t="s" s="2">
         <v>44</v>
@@ -8060,7 +8053,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -8176,11 +8169,11 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" t="s" s="2">
@@ -8199,16 +8192,16 @@
         <v>53</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="K57" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="L57" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>418</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>419</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -8258,7 +8251,7 @@
         <v>44</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -8273,16 +8266,16 @@
         <v>64</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="AK57" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="AK57" t="s" s="2">
+      <c r="AL57" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="AL57" t="s" s="2">
-        <v>422</v>
-      </c>
       <c r="AM57" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>44</v>
@@ -8290,7 +8283,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8316,10 +8309,10 @@
         <v>151</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -8346,14 +8339,14 @@
         <v>44</v>
       </c>
       <c r="W58" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X58" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="Y58" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="Y58" t="s" s="2">
-        <v>427</v>
-      </c>
       <c r="Z58" t="s" s="2">
         <v>44</v>
       </c>
@@ -8370,7 +8363,7 @@
         <v>44</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>42</v>
@@ -8391,10 +8384,10 @@
         <v>44</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>44</v>
@@ -8402,7 +8395,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8425,13 +8418,13 @@
         <v>53</v>
       </c>
       <c r="J59" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="K59" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="K59" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -8482,7 +8475,7 @@
         <v>44</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>42</v>
@@ -8503,10 +8496,10 @@
         <v>44</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>44</v>
@@ -8514,7 +8507,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8540,13 +8533,13 @@
         <v>151</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>435</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>436</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" t="s" s="2">
@@ -8572,14 +8565,14 @@
         <v>44</v>
       </c>
       <c r="W60" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X60" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="Y60" t="s" s="2">
         <v>437</v>
       </c>
-      <c r="Y60" t="s" s="2">
-        <v>438</v>
-      </c>
       <c r="Z60" t="s" s="2">
         <v>44</v>
       </c>
@@ -8596,7 +8589,7 @@
         <v>44</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8611,16 +8604,16 @@
         <v>64</v>
       </c>
       <c r="AJ60" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="AK60" t="s" s="2">
         <v>439</v>
       </c>
-      <c r="AK60" t="s" s="2">
+      <c r="AL60" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="AL60" t="s" s="2">
+      <c r="AM60" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>44</v>
@@ -8628,7 +8621,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8651,16 +8644,16 @@
         <v>53</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>444</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
@@ -8710,7 +8703,7 @@
         <v>44</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8725,16 +8718,16 @@
         <v>64</v>
       </c>
       <c r="AJ61" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="AK61" t="s" s="2">
         <v>448</v>
       </c>
-      <c r="AK61" t="s" s="2">
+      <c r="AL61" t="s" s="2">
         <v>449</v>
       </c>
-      <c r="AL61" t="s" s="2">
-        <v>450</v>
-      </c>
       <c r="AM61" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AN61" t="s" s="2">
         <v>44</v>
@@ -8742,7 +8735,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8765,13 +8758,13 @@
         <v>44</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>452</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>453</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>454</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -8822,7 +8815,7 @@
         <v>44</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>42</v>
@@ -8837,13 +8830,13 @@
         <v>64</v>
       </c>
       <c r="AJ62" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="AK62" t="s" s="2">
         <v>455</v>
       </c>
-      <c r="AK62" t="s" s="2">
+      <c r="AL62" t="s" s="2">
         <v>456</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>457</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>44</v>
@@ -8854,11 +8847,11 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" t="s" s="2">
@@ -8877,16 +8870,16 @@
         <v>44</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>460</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>461</v>
       </c>
-      <c r="L63" t="s" s="2">
+      <c r="M63" t="s" s="2">
         <v>462</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>463</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" t="s" s="2">
@@ -8936,7 +8929,7 @@
         <v>44</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>42</v>
@@ -8951,13 +8944,13 @@
         <v>64</v>
       </c>
       <c r="AJ63" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="AK63" t="s" s="2">
         <v>464</v>
       </c>
-      <c r="AK63" t="s" s="2">
+      <c r="AL63" t="s" s="2">
         <v>465</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>466</v>
       </c>
       <c r="AM63" t="s" s="2">
         <v>44</v>
@@ -8968,7 +8961,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8991,16 +8984,16 @@
         <v>53</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>468</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>469</v>
       </c>
-      <c r="L64" t="s" s="2">
+      <c r="M64" t="s" s="2">
         <v>470</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>471</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" t="s" s="2">
@@ -9050,7 +9043,7 @@
         <v>44</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>42</v>
@@ -9068,10 +9061,10 @@
         <v>44</v>
       </c>
       <c r="AK64" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AL64" t="s" s="2">
         <v>472</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>473</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>44</v>
@@ -9082,11 +9075,11 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" t="s" s="2">
@@ -9108,16 +9101,16 @@
         <v>151</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>476</v>
       </c>
-      <c r="L65" t="s" s="2">
+      <c r="M65" t="s" s="2">
         <v>477</v>
       </c>
-      <c r="M65" t="s" s="2">
+      <c r="N65" t="s" s="2">
         <v>478</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>479</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>44</v>
@@ -9142,14 +9135,14 @@
         <v>44</v>
       </c>
       <c r="W65" t="s" s="2">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X65" t="s" s="2">
+        <v>479</v>
+      </c>
+      <c r="Y65" t="s" s="2">
         <v>480</v>
       </c>
-      <c r="Y65" t="s" s="2">
-        <v>481</v>
-      </c>
       <c r="Z65" t="s" s="2">
         <v>44</v>
       </c>
@@ -9166,7 +9159,7 @@
         <v>44</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>42</v>
@@ -9184,21 +9177,21 @@
         <v>44</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AL65" t="s" s="2">
+        <v>481</v>
+      </c>
+      <c r="AM65" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN65" t="s" s="2">
         <v>482</v>
-      </c>
-      <c r="AM65" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN65" t="s" s="2">
-        <v>483</v>
       </c>
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9221,13 +9214,13 @@
         <v>44</v>
       </c>
       <c r="J66" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K66" t="s" s="2">
         <v>12</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
@@ -9278,7 +9271,7 @@
         <v>44</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>42</v>
@@ -9293,24 +9286,24 @@
         <v>64</v>
       </c>
       <c r="AJ66" t="s" s="2">
+        <v>486</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AL66" t="s" s="2">
         <v>487</v>
       </c>
-      <c r="AK66" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="AL66" t="s" s="2">
+      <c r="AM66" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN66" t="s" s="2">
         <v>488</v>
-      </c>
-      <c r="AM66" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN66" t="s" s="2">
-        <v>489</v>
       </c>
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9336,10 +9329,10 @@
         <v>54</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>490</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>491</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>492</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -9390,7 +9383,7 @@
         <v>44</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>42</v>
@@ -9408,10 +9401,10 @@
         <v>44</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>44</v>
@@ -9422,7 +9415,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9445,16 +9438,16 @@
         <v>44</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>494</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>495</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>496</v>
       </c>
-      <c r="L68" t="s" s="2">
+      <c r="M68" t="s" s="2">
         <v>497</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>498</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" t="s" s="2">
@@ -9504,7 +9497,7 @@
         <v>44</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>42</v>
@@ -9519,13 +9512,13 @@
         <v>64</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>95</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>44</v>

</xml_diff>